<commit_message>
Ajuste no layout e outras informações
</commit_message>
<xml_diff>
--- a/controle de multas planilha 3.xlsx
+++ b/controle de multas planilha 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seesp-my.sharepoint.com/personal/bruno_vargas_educacao_sp_gov_br/Documents/Grafico Roberto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.vargas\Desktop\PROJETOS\dashboard-dtran-nov25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{3FAAC6E3-EB51-4F86-86CE-F072A0165421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3170C5A5-1B1B-4477-B030-35C823714442}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A73E590-8F49-4DBC-99A2-88BAC7F75BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C98C8073-3913-44ED-9ABC-F58863568FC8}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C98C8073-3913-44ED-9ABC-F58863568FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="13" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="207">
   <si>
     <t>DIRETORIA</t>
-  </si>
-  <si>
-    <t>Multa/Notificação</t>
   </si>
   <si>
     <t xml:space="preserve">PLACA </t>
@@ -666,8 +663,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -695,8 +700,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,7 +1021,7 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G88"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,2026 +1036,2026 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2">
         <v>1234578392</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3">
         <v>1435797300</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4">
         <v>1331650094</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
         <v>111</v>
       </c>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5">
         <v>1430123483</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6">
         <v>1430123483</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <v>1255735136</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" t="s">
         <v>98</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" t="s">
-        <v>99</v>
-      </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>1255735136</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9">
         <v>1246366751</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <v>1246366751</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>1246366751</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12">
         <v>1328712564</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13">
         <v>1328712564</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
         <v>101</v>
       </c>
-      <c r="D14" t="s">
-        <v>102</v>
-      </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14">
         <v>598323600</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15">
         <v>598323600</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <v>598323600</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17">
         <v>598323600</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
         <v>107</v>
       </c>
-      <c r="D18" t="s">
-        <v>108</v>
-      </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18">
         <v>1000838240</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19">
         <v>1000838240</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
         <v>96</v>
       </c>
-      <c r="D20" t="s">
-        <v>97</v>
-      </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20">
         <v>1328713013</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21">
         <v>1255307495</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22">
         <v>1200104304</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
         <v>109</v>
       </c>
-      <c r="D23" t="s">
-        <v>110</v>
-      </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23">
         <v>1302983366</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24">
         <v>602965187</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F25">
         <v>1436987188</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" t="s">
         <v>91</v>
       </c>
-      <c r="D26" t="s">
-        <v>92</v>
-      </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F26">
         <v>1301135604</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F27">
         <v>1246344839</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>45979</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28">
         <v>1122675558</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29">
         <v>998538736</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F30">
         <v>1301133695</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F31">
         <v>1173309419</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F32">
         <v>994736304</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="D33" t="s">
-        <v>81</v>
-      </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F33">
         <v>13119624143</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F34">
         <v>1339038207</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35">
         <v>1200110932</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" t="s">
         <v>165</v>
       </c>
-      <c r="D36" t="s">
-        <v>166</v>
-      </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F36">
         <v>1246432185</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
         <v>84</v>
       </c>
-      <c r="D37" t="s">
-        <v>85</v>
-      </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F37">
         <v>1251921199</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" t="s">
         <v>82</v>
       </c>
-      <c r="D38" t="s">
-        <v>83</v>
-      </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38">
         <v>1324437658</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
         <v>86</v>
       </c>
-      <c r="D39" t="s">
-        <v>87</v>
-      </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F39">
         <v>1302911071</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" t="s">
         <v>167</v>
       </c>
-      <c r="D40" t="s">
-        <v>168</v>
-      </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F40">
         <v>1173307122</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F41">
         <v>1173307122</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42">
         <v>1343234490</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F43">
         <v>1343234490</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F44">
         <v>1255722964</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="2">
         <v>45986</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F45">
         <v>1173307122</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F46">
         <v>597898545</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F47">
         <v>597898545</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" t="s">
         <v>7</v>
-      </c>
-      <c r="C48" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" t="s">
-        <v>172</v>
-      </c>
-      <c r="E48" t="s">
-        <v>8</v>
       </c>
       <c r="F48">
         <v>992449553</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F49">
         <v>1246513630</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D50">
         <v>1341877997</v>
       </c>
       <c r="E50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F50">
         <v>1341877997</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" t="s">
         <v>132</v>
       </c>
-      <c r="D51" t="s">
-        <v>133</v>
-      </c>
       <c r="E51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F51">
         <v>1219733501</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" t="s">
         <v>129</v>
       </c>
-      <c r="D52" t="s">
-        <v>130</v>
-      </c>
       <c r="E52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F52">
         <v>1341877997</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F53">
         <v>1228549092</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F54">
         <v>1228549092</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
         <v>52</v>
       </c>
-      <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
-        <v>53</v>
-      </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F55">
         <v>1251987920</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
         <v>52</v>
       </c>
-      <c r="B56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
-        <v>53</v>
-      </c>
       <c r="D56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F56">
         <v>1251987920</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F57">
         <v>1228584394</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F58">
         <v>191966860</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
+        <v>175</v>
+      </c>
+      <c r="D59" t="s">
         <v>176</v>
       </c>
-      <c r="D59" t="s">
-        <v>177</v>
-      </c>
       <c r="E59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F59">
         <v>1321195467</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F60">
         <v>1232577208</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
         <v>32</v>
       </c>
-      <c r="B61" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s">
-        <v>33</v>
-      </c>
       <c r="D61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F61">
         <v>134620848</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" t="s">
         <v>181</v>
       </c>
-      <c r="D62" t="s">
-        <v>182</v>
-      </c>
       <c r="E62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F62">
         <v>1325596504</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" t="s">
         <v>7</v>
-      </c>
-      <c r="C63" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" t="s">
-        <v>74</v>
-      </c>
-      <c r="E63" t="s">
-        <v>8</v>
       </c>
       <c r="F63">
         <v>1301629615</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" t="s">
         <v>183</v>
       </c>
-      <c r="D64" t="s">
-        <v>184</v>
-      </c>
       <c r="E64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F64">
         <v>1219732602</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
+        <v>184</v>
+      </c>
+      <c r="D65" t="s">
         <v>185</v>
       </c>
-      <c r="D65" t="s">
-        <v>186</v>
-      </c>
       <c r="E65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F65">
         <v>1219732602</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F66">
         <v>1173308269</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D67">
         <v>1246218396</v>
       </c>
       <c r="E67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F67">
         <v>1246218396</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F68">
         <v>1297083919</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>45</v>
+      </c>
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
         <v>46</v>
       </c>
-      <c r="B69" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" t="s">
-        <v>47</v>
-      </c>
       <c r="D69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F69">
         <v>1246351517</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F70">
         <v>99853736</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D71" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F71">
         <v>1328712831</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D72" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F72">
         <v>1232574519</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F73">
         <v>1430048368</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E74" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F74">
         <v>1325595818</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="s">
         <v>29</v>
       </c>
-      <c r="B75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s">
-        <v>30</v>
-      </c>
       <c r="D75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F75">
         <v>1302910210</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
+        <v>121</v>
+      </c>
+      <c r="D76" t="s">
         <v>122</v>
       </c>
-      <c r="D76" t="s">
-        <v>123</v>
-      </c>
       <c r="E76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F76">
         <v>1234651278</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F77">
         <v>1316749506</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
+        <v>117</v>
+      </c>
+      <c r="D78" t="s">
         <v>118</v>
       </c>
-      <c r="D78" t="s">
-        <v>119</v>
-      </c>
       <c r="E78" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F78">
         <v>1316749506</v>
       </c>
-      <c r="G78">
+      <c r="G78" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E79" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F79">
         <v>1321194010</v>
       </c>
-      <c r="G79">
+      <c r="G79" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>196</v>
+      </c>
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" t="s">
         <v>197</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
+        <v>198</v>
+      </c>
+      <c r="E80" t="s">
         <v>7</v>
-      </c>
-      <c r="C80" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" t="s">
-        <v>199</v>
-      </c>
-      <c r="E80" t="s">
-        <v>8</v>
       </c>
       <c r="F80">
         <v>1005578408</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D81" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E81" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F81">
         <v>1319702500</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E82" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F82">
         <v>1232575566</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
+        <v>140</v>
+      </c>
+      <c r="D83" t="s">
         <v>141</v>
       </c>
-      <c r="D83" t="s">
-        <v>142</v>
-      </c>
       <c r="E83" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F83">
         <v>1251988285</v>
       </c>
-      <c r="G83">
+      <c r="G83" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" t="s">
+        <v>137</v>
+      </c>
+      <c r="D84" t="s">
+        <v>138</v>
+      </c>
+      <c r="E84" t="s">
         <v>7</v>
-      </c>
-      <c r="C84" t="s">
-        <v>138</v>
-      </c>
-      <c r="D84" t="s">
-        <v>139</v>
-      </c>
-      <c r="E84" t="s">
-        <v>8</v>
       </c>
       <c r="F84">
         <v>996972595</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D85" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E85" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F85">
         <v>1302979903</v>
       </c>
-      <c r="G85">
+      <c r="G85" s="2">
         <v>45988</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
+        <v>202</v>
+      </c>
+      <c r="D86" t="s">
         <v>203</v>
       </c>
-      <c r="D86" t="s">
-        <v>204</v>
-      </c>
       <c r="E86" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F86">
         <v>1321194010</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="2">
         <v>45989</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
+        <v>204</v>
+      </c>
+      <c r="D87" t="s">
         <v>205</v>
       </c>
-      <c r="D87" t="s">
-        <v>206</v>
-      </c>
       <c r="E87" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F87">
         <v>1316749506</v>
       </c>
-      <c r="G87">
+      <c r="G87" s="2">
         <v>45989</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D88" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E88" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F88">
         <v>1200457258</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="2">
         <v>45989</v>
       </c>
     </row>

</xml_diff>